<commit_message>
hash file colums added mongo db
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,6 +1,126 @@
 
-<file path=theme/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karani\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637C526D-0519-40C9-9557-A8E8103B3088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="sayfa1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Ürün</t>
+  </si>
+  <si>
+    <t>Müşteri</t>
+  </si>
+  <si>
+    <t>Toplam Satılan Mal</t>
+  </si>
+  <si>
+    <t>Toplam Fiyat</t>
+  </si>
+  <si>
+    <t>Satıldığı Tarih</t>
+  </si>
+  <si>
+    <t>Bilgisayar</t>
+  </si>
+  <si>
+    <t>Masaüstü Bilgisayar</t>
+  </si>
+  <si>
+    <t>Klavye</t>
+  </si>
+  <si>
+    <t>Modem</t>
+  </si>
+  <si>
+    <t>Ahmet</t>
+  </si>
+  <si>
+    <t>Mehmet</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Hasan</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -42,7 +162,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -77,7 +197,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,9 +371,118 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
-<file path=theme/theme/themeManager.xml><?xml version="1.0" encoding="utf-8"?>
-<a:themeManager xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+      <c r="D3">
+        <v>20000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43844</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>5000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43966</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>6000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>